<commit_message>
deeprange write record to excel named range
dynamically dimension an arry; use it to initialize a record with a named field; the record's name must be a substring of the field name; use record to fill named range inside excel spreadsheet but using the runtime variable of the data to be acquaried.
</commit_message>
<xml_diff>
--- a/deeprange.xlsx
+++ b/deeprange.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapplen\Documents\GitHub\sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73EFF495-945C-4A2A-9871-AC7426734DBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159084B8-2CEB-43B5-9F69-1BE2FE8FF90F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD21DE5B-1783-4FAC-BA3B-B8CA03FEC6B8}"/>
+    <workbookView xWindow="825" yWindow="1095" windowWidth="26355" windowHeight="13620" xr2:uid="{CD21DE5B-1783-4FAC-BA3B-B8CA03FEC6B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="band1_nf" localSheetId="0">Sheet1!$I$11</definedName>
+    <definedName name="band2_nf" localSheetId="0">Sheet1!$J$11</definedName>
     <definedName name="deeprange">Sheet1!$A$11:$A$101</definedName>
+    <definedName name="foo" localSheetId="0">Sheet1!$H$11</definedName>
     <definedName name="rangestart" localSheetId="0">Sheet1!$C$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -83,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>deeprange</t>
   </si>
@@ -101,6 +104,15 @@
   </si>
   <si>
     <t>now what</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>B2_nf</t>
+  </si>
+  <si>
+    <t>band1_nf</t>
   </si>
 </sst>
 </file>
@@ -511,12 +523,12 @@
   <dimension ref="A10:AT101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AT78" sqref="AT78"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -527,8 +539,17 @@
         <f t="array" aca="1" ref="F10" ca="1">CELL("address",rangestart)</f>
         <v>$C$11</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -540,7 +561,7 @@
         <v>$A$11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -548,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -556,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -564,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>

</xml_diff>